<commit_message>
evidence and dark patterns categories added
</commit_message>
<xml_diff>
--- a/datasets/patents_monitoring_tools.xlsx
+++ b/datasets/patents_monitoring_tools.xlsx
@@ -1209,7 +1209,7 @@
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>'behavioral profiling', 'targeted advertising'</t>
+          <t>'targeted advertising', 'behavioral profiling'</t>
         </is>
       </c>
     </row>
@@ -1659,7 +1659,7 @@
       </c>
       <c r="E52" t="inlineStr">
         <is>
-          <t>'behavioral profiling', 'targeted advertising'</t>
+          <t>'targeted advertising', 'behavioral profiling'</t>
         </is>
       </c>
     </row>
@@ -1734,7 +1734,7 @@
       </c>
       <c r="E55" t="inlineStr">
         <is>
-          <t>'behavioral profiling', 'targeted advertising'</t>
+          <t>'targeted advertising', 'behavioral profiling'</t>
         </is>
       </c>
     </row>
@@ -1834,7 +1834,7 @@
       </c>
       <c r="E59" t="inlineStr">
         <is>
-          <t>'behavioral profiling', 'targeted advertising'</t>
+          <t>'targeted advertising', 'behavioral profiling'</t>
         </is>
       </c>
     </row>

</xml_diff>